<commit_message>
Updated BOM: pin headers/Alternative Arduino
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\Fiero Headlight Controller\KiCAD Remake Public Release\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6439EA4-7958-4C33-8254-95A77C095BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F276F78E-EE67-4E64-A93C-D239AAA495B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="73">
   <si>
     <t>Component</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>Arduino Nano</t>
-  </si>
-  <si>
-    <t>Cheaper third-party alternatives are available, if you trust them.</t>
   </si>
   <si>
     <t>HiLetgo 2pcs ACS712 30A
@@ -263,6 +260,22 @@
       <t>Requiures a crimper such as https://www.amazon.com/dp/B08CZDRV4N
 A normal butt splice crimper will not work for these!</t>
     </r>
+  </si>
+  <si>
+    <t>Cheaper third-party alternatives are available, if you trust them.
+I personally used this clone board: https://www.amazon.com/dp/B09KGVDXZY</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B08DVGCTKT</t>
+  </si>
+  <si>
+    <t>2.54mm Breakaway Header/Pins</t>
+  </si>
+  <si>
+    <t>A1, U2, U3</t>
+  </si>
+  <si>
+    <t>Used to socket the Arduino and also to mount the current sensors. For current sensors, you will use 4 segments of 3-pin connector. For two of them, remove the middle pin. You'll see where they go.</t>
   </si>
 </sst>
 </file>
@@ -349,7 +362,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -366,6 +379,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -648,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="A18" sqref="A18:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,7 +681,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -676,7 +692,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
@@ -685,7 +701,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -693,331 +709,348 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>6</v>
+      <c r="E3" s="11" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="5">
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="5">
         <v>4</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2">
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="5">
         <v>8</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2">
         <v>4</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="5">
         <v>7</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="2">
         <v>3</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="5">
         <v>4</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="2">
         <v>1</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="5">
         <v>2</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="2">
         <v>1</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="5">
         <v>1</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="5">
+        <v>1</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+    </row>
+    <row r="19" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="4" t="s">
+      <c r="D20" s="8" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-    </row>
-    <row r="18" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="E20" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="2">
-        <v>1</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="B21" s="5">
+        <v>1</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="D21" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="E21" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="5">
-        <v>1</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="6" t="s">
+      <c r="D22" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="5">
+        <v>1</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="E23" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24">
+        <v>10</v>
+      </c>
+      <c r="C24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="5">
-        <v>1</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23">
-        <v>10</v>
-      </c>
-      <c r="C23" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>68</v>
+      <c r="E24" s="9" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A18:D18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D16" r:id="rId1" xr:uid="{168D27C3-D85D-4837-8BF2-C813567B5BE1}"/>
@@ -1034,11 +1067,11 @@
     <hyperlink ref="D5" r:id="rId12" xr:uid="{8AB57890-5588-42ED-898F-7FD93F68DA55}"/>
     <hyperlink ref="D4" r:id="rId13" xr:uid="{5339FCCC-062A-4047-B4E5-B4195DECE756}"/>
     <hyperlink ref="D3" r:id="rId14" xr:uid="{6C4EB022-E7FA-4E86-87B8-1DAE8FF11132}"/>
-    <hyperlink ref="D19" r:id="rId15" xr:uid="{C9F09EE5-4D5F-40C8-BF69-F851F18AFBA4}"/>
-    <hyperlink ref="D20" r:id="rId16" xr:uid="{7631671A-0B61-44AF-9DFD-ACC4C1E437D4}"/>
-    <hyperlink ref="D22" r:id="rId17" xr:uid="{3AD99C84-DEFB-4283-A663-909043A150DD}"/>
-    <hyperlink ref="D21" r:id="rId18" xr:uid="{EF288CC0-F754-4DFD-B4C6-F6F8CA60D93E}"/>
-    <hyperlink ref="D23" r:id="rId19" xr:uid="{FA3BCAF8-C9DF-4B44-B7FC-31260C2635F4}"/>
+    <hyperlink ref="D20" r:id="rId15" xr:uid="{C9F09EE5-4D5F-40C8-BF69-F851F18AFBA4}"/>
+    <hyperlink ref="D21" r:id="rId16" xr:uid="{7631671A-0B61-44AF-9DFD-ACC4C1E437D4}"/>
+    <hyperlink ref="D23" r:id="rId17" xr:uid="{3AD99C84-DEFB-4283-A663-909043A150DD}"/>
+    <hyperlink ref="D22" r:id="rId18" xr:uid="{EF288CC0-F754-4DFD-B4C6-F6F8CA60D93E}"/>
+    <hyperlink ref="D24" r:id="rId19" xr:uid="{FA3BCAF8-C9DF-4B44-B7FC-31260C2635F4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>